<commit_message>
delete samples for running faster
</commit_message>
<xml_diff>
--- a/example/example_expression_info.xlsx
+++ b/example/example_expression_info.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -23,7 +23,7 @@
     <t xml:space="preserve">AFP</t>
   </si>
   <si>
-    <t xml:space="preserve">T1013</t>
+    <t xml:space="preserve">T1021</t>
   </si>
   <si>
     <t xml:space="preserve">I</t>
@@ -32,34 +32,22 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">T1015</t>
+    <t xml:space="preserve">T1025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T1027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">III+IV</t>
   </si>
   <si>
     <t xml:space="preserve">0</t>
   </si>
   <si>
-    <t xml:space="preserve">T1021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T1025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T1027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">III+IV</t>
-  </si>
-  <si>
     <t xml:space="preserve">T1031</t>
   </si>
   <si>
     <t xml:space="preserve">T1041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T1043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T112</t>
   </si>
   <si>
     <t xml:space="preserve">T113</t>
@@ -424,23 +412,23 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -451,13 +439,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -465,54 +453,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>